<commit_message>
USART2 tööle. Sensorite andmed saadetakse arvutisse üle xRF-i. NB! Korraga saab hetkel töös olla ainult üks UART/USART.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,10 +1056,10 @@
       <c r="A13" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>71</v>
       </c>
       <c r="F13" t="s">

</xml_diff>

<commit_message>
Tugi 8 URF anduri jaoks. Hetkel kõik veel ei tööta. CAN protokoll sai dokumendis muudetud, vaja koodis ka muudatusi teha.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="140">
   <si>
     <t>STM32 pinout</t>
   </si>
@@ -412,6 +412,30 @@
   </si>
   <si>
     <t>USART2_RX / XRF_Rx</t>
+  </si>
+  <si>
+    <t>URF5 echo</t>
+  </si>
+  <si>
+    <t>URF6 echo</t>
+  </si>
+  <si>
+    <t>URF7 echo</t>
+  </si>
+  <si>
+    <t>URF8 echo</t>
+  </si>
+  <si>
+    <t>URF5 trig</t>
+  </si>
+  <si>
+    <t>URF6 trig</t>
+  </si>
+  <si>
+    <t>URF7 trig</t>
+  </si>
+  <si>
+    <t>URF8 trig</t>
   </si>
 </sst>
 </file>
@@ -873,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,12 +1158,18 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="F16" t="s">
+        <v>136</v>
+      </c>
       <c r="G16" s="6" t="s">
         <v>113</v>
       </c>
@@ -1153,12 +1183,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>75</v>
+      </c>
+      <c r="F17" t="s">
+        <v>137</v>
       </c>
       <c r="G17" s="6"/>
       <c r="I17" s="1" t="s">
@@ -1168,7 +1204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1186,12 +1222,18 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>77</v>
+      </c>
+      <c r="F19" t="s">
+        <v>138</v>
       </c>
       <c r="G19" s="6"/>
       <c r="I19" s="4" t="s">
@@ -1225,12 +1267,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>135</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>78</v>
+      </c>
+      <c r="F20" t="s">
+        <v>139</v>
       </c>
       <c r="G20" s="6"/>
       <c r="I20" s="4" t="s">
@@ -1258,7 +1306,7 @@
       <c r="T20" s="11"/>
       <c r="U20" s="13"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>57</v>
       </c>
@@ -1281,7 +1329,7 @@
       <c r="T21" s="11"/>
       <c r="U21" s="13"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>58</v>
       </c>
@@ -1307,7 +1355,7 @@
       <c r="T22" s="11"/>
       <c r="U22" s="13"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>59</v>
       </c>
@@ -1332,7 +1380,7 @@
       <c r="T23" s="11"/>
       <c r="U23" s="13"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>60</v>
       </c>
@@ -1358,7 +1406,7 @@
       <c r="T24" s="11"/>
       <c r="U24" s="13"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>61</v>
       </c>
@@ -1391,7 +1439,7 @@
       <c r="T25" s="11"/>
       <c r="U25" s="13"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
         <v>62</v>
       </c>
@@ -1414,7 +1462,7 @@
       <c r="T26" s="11"/>
       <c r="U26" s="13"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>63</v>
       </c>
@@ -1437,7 +1485,7 @@
       <c r="T27" s="11"/>
       <c r="U27" s="13"/>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
         <v>64</v>
       </c>
@@ -1463,7 +1511,7 @@
       <c r="T28" s="11"/>
       <c r="U28" s="13"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>95</v>
       </c>
@@ -1492,7 +1540,7 @@
       <c r="T29" s="11"/>
       <c r="U29" s="13"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>96</v>
       </c>
@@ -1518,7 +1566,7 @@
       <c r="T30" s="11"/>
       <c r="U30" s="13"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
8 URF sensorit tööle.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -898,7 +898,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,10 +1161,10 @@
       <c r="A16" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>74</v>
       </c>
       <c r="F16" t="s">
@@ -1187,10 +1187,10 @@
       <c r="A17" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>75</v>
       </c>
       <c r="F17" t="s">
@@ -1226,10 +1226,10 @@
       <c r="A19" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F19" t="s">
@@ -1271,10 +1271,10 @@
       <c r="A20" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F20" t="s">

</xml_diff>

<commit_message>
Mootorikontrollerites on kiiruse sõnumi timeout. Kui 10x perioodi jooksul pole kiiruse sõnumit tulnud, siis pannakse mootorid seisma. Parandatud CAN sõnumite vastuvõtmine sensori plaadil (STm32F4 kit). Mootorite kiiruste kuvamine UI-s. Kiiruse seadmine O ja I klahvide alt.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
   <si>
     <t>STM32 pinout</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>URF8 trig</t>
+  </si>
+  <si>
+    <t>acceler SPI</t>
   </si>
 </sst>
 </file>
@@ -897,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1112,9 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>51</v>
       </c>
@@ -1135,13 +1141,18 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="6"/>
       <c r="H15" t="s">

</xml_diff>

<commit_message>
Parandused URF sensorite lugemises.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="13395" windowHeight="4935"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="4875"/>
   </bookViews>
   <sheets>
     <sheet name="STM32" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
   <si>
     <t>STM32 pinout</t>
   </si>
@@ -439,6 +439,18 @@
   </si>
   <si>
     <t>acceler SPI</t>
+  </si>
+  <si>
+    <t>I2C3_SCL</t>
+  </si>
+  <si>
+    <t>I2C3_SDA</t>
+  </si>
+  <si>
+    <t>Vbus green LED</t>
+  </si>
+  <si>
+    <t>CS43L22 MCLK</t>
   </si>
 </sst>
 </file>
@@ -900,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,11 +1519,17 @@
         <v>93</v>
       </c>
       <c r="G28" s="6"/>
+      <c r="H28" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I28" s="4" t="s">
         <v>33</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="11"/>
@@ -1542,6 +1560,9 @@
       <c r="J29" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="K29" t="s">
+        <v>142</v>
+      </c>
       <c r="N29" s="6"/>
       <c r="O29" s="11"/>
       <c r="P29" s="6"/>
@@ -1567,6 +1588,9 @@
       </c>
       <c r="J30" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="K30" t="s">
+        <v>144</v>
       </c>
       <c r="N30" s="6"/>
       <c r="O30" s="11"/>

</xml_diff>

<commit_message>
VisionBoard edastab CAN-i Pixy kaameras leitud objekti.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1522,7 @@
       <c r="H28" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="5" t="s">
         <v>33</v>
       </c>
       <c r="J28" s="1" t="s">
@@ -1557,7 +1557,7 @@
       <c r="I29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="5" t="s">
         <v>44</v>
       </c>
       <c r="K29" t="s">

</xml_diff>

<commit_message>
Akumooduliga suhtlemiseks on I2C1 ja I2C3.
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="146">
   <si>
     <t>STM32 pinout</t>
   </si>
@@ -333,9 +333,6 @@
     <t>CAN1_Tx</t>
   </si>
   <si>
-    <t>SDA</t>
-  </si>
-  <si>
     <t>kit function</t>
   </si>
   <si>
@@ -451,6 +448,12 @@
   </si>
   <si>
     <t>CS43L22 MCLK</t>
+  </si>
+  <si>
+    <t>I2C1_SCL</t>
+  </si>
+  <si>
+    <t>I2C1_SDA</t>
   </si>
 </sst>
 </file>
@@ -912,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +951,7 @@
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J4" s="2"/>
       <c r="K4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -961,7 +964,7 @@
         <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
         <v>101</v>
@@ -970,10 +973,10 @@
         <v>101</v>
       </c>
       <c r="H6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L6" t="s">
         <v>101</v>
@@ -1053,7 +1056,7 @@
         <v>69</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>6</v>
@@ -1062,7 +1065,7 @@
         <v>14</v>
       </c>
       <c r="L11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1076,7 +1079,7 @@
         <v>89</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>7</v>
@@ -1085,15 +1088,15 @@
         <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>50</v>
@@ -1102,10 +1105,10 @@
         <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>8</v>
@@ -1114,18 +1117,18 @@
         <v>16</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>51</v>
@@ -1134,7 +1137,7 @@
         <v>72</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>9</v>
@@ -1146,15 +1149,15 @@
         <v>97</v>
       </c>
       <c r="P14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>52</v>
@@ -1163,12 +1166,12 @@
         <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="6"/>
       <c r="H15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>10</v>
@@ -1177,12 +1180,12 @@
         <v>18</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>53</v>
@@ -1191,24 +1194,24 @@
         <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>54</v>
@@ -1217,7 +1220,7 @@
         <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G17" s="6"/>
       <c r="I17" s="1" t="s">
@@ -1235,19 +1238,22 @@
         <v>76</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="I18" s="1" t="s">
+      <c r="H18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="P18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>55</v>
@@ -1256,7 +1262,7 @@
         <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G19" s="6"/>
       <c r="I19" s="4" t="s">
@@ -1292,7 +1298,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>56</v>
@@ -1301,7 +1307,7 @@
         <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G20" s="6"/>
       <c r="I20" s="4" t="s">
@@ -1311,20 +1317,20 @@
         <v>22</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O20" s="11"/>
       <c r="P20" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q20" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q20" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="R20" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T20" s="11"/>
       <c r="U20" s="13"/>
@@ -1440,7 +1446,7 @@
         <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>30</v>
@@ -1455,7 +1461,7 @@
       <c r="O25" s="11"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R25" s="11"/>
       <c r="S25" s="13"/>
@@ -1520,7 +1526,7 @@
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>33</v>
@@ -1529,7 +1535,7 @@
         <v>43</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="11"/>
@@ -1561,7 +1567,7 @@
         <v>44</v>
       </c>
       <c r="K29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="11"/>
@@ -1590,7 +1596,7 @@
         <v>45</v>
       </c>
       <c r="K30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N30" s="6"/>
       <c r="O30" s="11"/>

</xml_diff>

<commit_message>
Updated sensor board pinout document with stop button
</commit_message>
<xml_diff>
--- a/Software/LowLevel/Documents/STM32_pinout.xlsx
+++ b/Software/LowLevel/Documents/STM32_pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="147">
   <si>
     <t>STM32 pinout</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>I2C1_SDA</t>
+  </si>
+  <si>
+    <t>stop switch</t>
   </si>
 </sst>
 </file>
@@ -915,19 +918,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.75" customWidth="1"/>
+    <col min="11" max="11" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1559,8 +1562,10 @@
       <c r="E29" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="I29" s="4" t="s">
+      <c r="G29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="I29" s="5" t="s">
         <v>34</v>
       </c>
       <c r="J29" s="5" t="s">

</xml_diff>